<commit_message>
Adicionado o Documento Oficial e atualizado o excel dos Requisitos F e NF
</commit_message>
<xml_diff>
--- a/Documentos/excel/RequisitosDoProjeto.xlsx
+++ b/Documentos/excel/RequisitosDoProjeto.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cliente\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alunos\Desktop\Fatec_Matheus\PI\Projeto_Interdisciplinar\Documentos\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98C15989-AB5C-47B1-9BEA-0756B579641E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{790F6D4B-D6FA-4DD0-81FA-2F1787108237}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10440" xr2:uid="{BA98B352-8331-4BCF-9395-F3BA140B09FC}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{BA98B352-8331-4BCF-9395-F3BA140B09FC}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -20,22 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="103">
   <si>
     <t>Nº Requisito</t>
   </si>
@@ -256,9 +246,6 @@
     <t>link para a página de reclamações</t>
   </si>
   <si>
-    <t>haverá no footer um link direcionando o usuário para a página de reclamações</t>
-  </si>
-  <si>
     <t>RF016</t>
   </si>
   <si>
@@ -274,57 +261,89 @@
     <t>link para a página de reclamações filtradas por bairro</t>
   </si>
   <si>
-    <t>haverá no footer um link direcionando o usuário para a página busca por bairro</t>
-  </si>
-  <si>
     <t>RF018</t>
   </si>
   <si>
     <t>link para a pagina de orgãos responsaveis</t>
   </si>
   <si>
-    <t>haverá no footer um link direcionando o usuário para a página de orgãos responsáveis</t>
-  </si>
-  <si>
     <t>RF019</t>
   </si>
   <si>
     <t>link para a página de doenças relacionadas</t>
   </si>
   <si>
-    <t>haverá no footer um link direcionando o usuário para a página de doenças relacionadas</t>
-  </si>
-  <si>
     <t>RF020</t>
   </si>
   <si>
     <t>links para as redes sociais do site</t>
   </si>
   <si>
-    <t>haverá no footer links para as redes sociais do site</t>
-  </si>
-  <si>
     <t>S</t>
   </si>
   <si>
     <t>O site deverá ter acessibilidade para daltonicos, cegos , pessoas com visão debilitada e gerais.</t>
+  </si>
+  <si>
+    <t>Cadastro de Doenças</t>
+  </si>
+  <si>
+    <t>O usuário administrador poderá registrar informações sobre uma determinada doença e adicionar a lista de doenças do site</t>
+  </si>
+  <si>
+    <t>RF021</t>
+  </si>
+  <si>
+    <t>RF022</t>
+  </si>
+  <si>
+    <t>Cadastro de Notícias</t>
+  </si>
+  <si>
+    <t>O usuário administrador poderá registrar informações sobre uma determinada notícia e adicionar a lista de notícias do site</t>
+  </si>
+  <si>
+    <t>Haverá no footer um link direcionando o usuário para a página busca por bairro</t>
+  </si>
+  <si>
+    <t>Haverá no footer um link direcionando o usuário para a página de reclamações</t>
+  </si>
+  <si>
+    <t>Haverá no footer um link direcionando o usuário para a página de orgãos responsáveis</t>
+  </si>
+  <si>
+    <t>Haverá no footer um link direcionando o usuário para a página de doenças relacionadas</t>
+  </si>
+  <si>
+    <t>Haverá no footer links para as redes sociais do site</t>
+  </si>
+  <si>
+    <t>RF023</t>
+  </si>
+  <si>
+    <t>Resposta à reclamação do Cliente</t>
+  </si>
+  <si>
+    <t>Uma reclamação pode receber uma resposta feita pelo usuário administrador</t>
+  </si>
+  <si>
+    <t>RF024</t>
+  </si>
+  <si>
+    <t>Réplica da resposta</t>
+  </si>
+  <si>
+    <t>Após receber uma resposta do administrador, o usuário pode realizar uma réplica, e receber outra resposta novamente</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -349,6 +368,18 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -383,7 +414,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -460,57 +491,72 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -830,469 +876,593 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30AA77CB-0655-4332-9862-3BB74B5B7403}">
-  <dimension ref="A1:H53"/>
+  <dimension ref="A1:H54"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="12.28515625" customWidth="1"/>
-    <col min="3" max="3" width="34.85546875" customWidth="1"/>
-    <col min="4" max="4" width="77.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.85546875" customWidth="1"/>
-    <col min="7" max="7" width="34.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="54.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.26953125" customWidth="1"/>
+    <col min="3" max="3" width="34.81640625" customWidth="1"/>
+    <col min="4" max="4" width="77.1796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.81640625" customWidth="1"/>
+    <col min="7" max="7" width="34.1796875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="54.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B3" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="9"/>
+      <c r="F3" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="28" x14ac:dyDescent="0.35">
+      <c r="B4" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="9"/>
+      <c r="F4" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="G4" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="H4" s="12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="28" x14ac:dyDescent="0.35">
+      <c r="B5" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="9"/>
+      <c r="F5" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="H5" s="14" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B6" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="9"/>
+      <c r="F6" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="G6" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="H6" s="12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="28" x14ac:dyDescent="0.35">
+      <c r="B7" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" s="9"/>
+      <c r="F7" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="G7" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="H7" s="17" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="42" x14ac:dyDescent="0.35">
+      <c r="B8" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="E8" s="9"/>
+      <c r="F8" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="G8" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="H8" s="12" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="42" x14ac:dyDescent="0.35">
+      <c r="B9" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="E9" s="9"/>
+      <c r="F9" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="G9" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="H9" s="17" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="28" x14ac:dyDescent="0.35">
+      <c r="B10" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="E10" s="9"/>
+      <c r="F10" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="G10" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="H10" s="12" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="28" x14ac:dyDescent="0.35">
+      <c r="B11" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="C11" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="D11" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="E11" s="9"/>
+      <c r="F11" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="G11" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="H11" s="17" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="42" x14ac:dyDescent="0.35">
+      <c r="B12" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="D12" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="E12" s="9"/>
+      <c r="F12" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="G12" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="H12" s="12" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="28" x14ac:dyDescent="0.35">
+      <c r="B13" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="C13" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="D13" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="9"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B14" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="D14" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="E14" s="9"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="9"/>
+    </row>
+    <row r="15" spans="1:8" ht="28" x14ac:dyDescent="0.35">
+      <c r="A15" s="2"/>
+      <c r="B15" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="C15" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="D15" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="9"/>
+      <c r="H15" s="9"/>
+    </row>
+    <row r="16" spans="1:8" ht="28" x14ac:dyDescent="0.35">
+      <c r="B16" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="D16" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="E16" s="9"/>
+      <c r="F16" s="9"/>
+      <c r="G16" s="9"/>
+      <c r="H16" s="9"/>
+    </row>
+    <row r="17" spans="2:8" ht="28" x14ac:dyDescent="0.35">
+      <c r="B17" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="C17" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="D17" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="E17" s="9"/>
+      <c r="F17" s="9"/>
+      <c r="G17" s="9"/>
+      <c r="H17" s="9"/>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B18" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="C18" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="D18" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="E18" s="9"/>
+      <c r="F18" s="9"/>
+      <c r="G18" s="9"/>
+      <c r="H18" s="9"/>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B19" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="C19" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="D19" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="E19" s="9"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="9"/>
+      <c r="H19" s="9"/>
+    </row>
+    <row r="20" spans="2:8" ht="28" x14ac:dyDescent="0.35">
+      <c r="B20" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="C20" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="D20" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="E20" s="9"/>
+      <c r="F20" s="9"/>
+      <c r="G20" s="9"/>
+      <c r="H20" s="9"/>
+    </row>
+    <row r="21" spans="2:8" ht="28" x14ac:dyDescent="0.35">
+      <c r="B21" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="C21" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="D21" s="18" t="s">
+        <v>94</v>
+      </c>
+      <c r="E21" s="9"/>
+      <c r="F21" s="9"/>
+      <c r="G21" s="9"/>
+      <c r="H21" s="9"/>
+    </row>
+    <row r="22" spans="2:8" ht="28" x14ac:dyDescent="0.35">
+      <c r="B22" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="C22" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="D22" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="E22" s="9"/>
+      <c r="F22" s="9"/>
+      <c r="G22" s="9"/>
+      <c r="H22" s="9"/>
+    </row>
+    <row r="23" spans="2:8" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B23" s="20" t="s">
+        <v>82</v>
+      </c>
+      <c r="C23" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="D23" s="21" t="s">
+        <v>96</v>
+      </c>
+      <c r="E23" s="9"/>
+      <c r="F23" s="9"/>
+      <c r="G23" s="9"/>
+      <c r="H23" s="9"/>
+    </row>
+    <row r="24" spans="2:8" ht="28" x14ac:dyDescent="0.35">
+      <c r="B24" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="C24" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="D24" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="E24" s="9"/>
+      <c r="F24" s="9"/>
+      <c r="G24" s="9"/>
+      <c r="H24" s="9"/>
+    </row>
+    <row r="25" spans="2:8" ht="28" x14ac:dyDescent="0.35">
+      <c r="B25" s="20" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B3" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="B4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H4" s="5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="B5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H5" s="7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="F6" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="H6" s="5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="B7" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="D7" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="F7" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="G7" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="H7" s="9" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="B8" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="F8" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="G8" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="H8" s="5" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="B9" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C9" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="D9" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="F9" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="G9" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="H9" s="9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="B10" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="F10" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="G10" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="H10" s="5" t="s">
+      <c r="C25" s="21" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="B11" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C11" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="D11" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="F11" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="G11" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="H11" s="9" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="B12" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="F12" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="G12" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="H12" s="5" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="B13" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C13" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="D13" s="9" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="B14" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="19"/>
-      <c r="B15" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="C15" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="D15" s="9" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="B16" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="17" spans="2:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B17" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="C17" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="D17" s="9" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B18" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B19" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="C19" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="D19" s="8" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="20" spans="2:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B20" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="21" spans="2:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B21" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="C21" s="11" t="s">
-        <v>81</v>
-      </c>
-      <c r="D21" s="11" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="22" spans="2:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B22" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="D22" s="5" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B23" s="17" t="s">
-        <v>86</v>
-      </c>
-      <c r="C23" s="18" t="s">
-        <v>87</v>
-      </c>
-      <c r="D23" s="18" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C28" s="12"/>
-    </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B35" s="13"/>
-      <c r="C35" s="13"/>
-      <c r="D35" s="13"/>
-    </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B36" s="13"/>
-      <c r="C36" s="14"/>
-      <c r="D36" s="14"/>
-    </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B37" s="13"/>
-      <c r="C37" s="14"/>
-      <c r="D37" s="14"/>
-    </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B38" s="15"/>
-      <c r="C38" s="14"/>
-      <c r="D38" s="16"/>
-    </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B39" s="13"/>
-      <c r="C39" s="14"/>
-      <c r="D39" s="16"/>
-    </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B40" s="13"/>
-      <c r="C40" s="14"/>
-      <c r="D40" s="16"/>
-    </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B41" s="13"/>
-      <c r="C41" s="14"/>
-      <c r="D41" s="16"/>
-    </row>
-    <row r="42" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B42" s="13"/>
-      <c r="C42" s="14"/>
-      <c r="D42" s="16"/>
-    </row>
-    <row r="43" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B43" s="13"/>
-      <c r="C43" s="14"/>
-      <c r="D43" s="16"/>
-    </row>
-    <row r="44" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B44" s="13"/>
-      <c r="C44" s="14"/>
-      <c r="D44" s="16"/>
-    </row>
-    <row r="45" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B45" s="13"/>
-      <c r="C45" s="14"/>
-      <c r="D45" s="16"/>
-    </row>
-    <row r="46" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B46" s="13"/>
-      <c r="C46" s="14"/>
-      <c r="D46" s="16"/>
-    </row>
-    <row r="47" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B47" s="13"/>
-      <c r="C47" s="14"/>
-      <c r="D47" s="16"/>
-    </row>
-    <row r="48" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B48" s="13"/>
-      <c r="C48" s="14"/>
-      <c r="D48" s="16"/>
-    </row>
-    <row r="49" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B49" s="13"/>
-      <c r="C49" s="14"/>
-      <c r="D49" s="16"/>
-    </row>
-    <row r="50" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B50" s="13"/>
-      <c r="C50" s="14"/>
-      <c r="D50" s="16"/>
-    </row>
-    <row r="51" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B51" s="13"/>
-      <c r="C51" s="14"/>
-      <c r="D51" s="16"/>
-    </row>
-    <row r="52" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B52" s="13"/>
-      <c r="C52" s="14"/>
-      <c r="D52" s="16"/>
-    </row>
-    <row r="53" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B53" s="13"/>
-      <c r="C53" s="14"/>
-      <c r="D53" s="16"/>
+      <c r="D25" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="E25" s="9"/>
+      <c r="F25" s="9"/>
+      <c r="G25" s="9"/>
+      <c r="H25" s="9"/>
+    </row>
+    <row r="26" spans="2:8" ht="21.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B26" s="19" t="s">
+        <v>97</v>
+      </c>
+      <c r="C26" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="D26" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="E26" s="9"/>
+      <c r="F26" s="9"/>
+      <c r="G26" s="9"/>
+      <c r="H26" s="9"/>
+    </row>
+    <row r="27" spans="2:8" ht="28" x14ac:dyDescent="0.35">
+      <c r="B27" s="20" t="s">
+        <v>100</v>
+      </c>
+      <c r="C27" s="21" t="s">
+        <v>101</v>
+      </c>
+      <c r="D27" s="21" t="s">
+        <v>102</v>
+      </c>
+      <c r="E27" s="9"/>
+      <c r="F27" s="9"/>
+      <c r="G27" s="9"/>
+      <c r="H27" s="9"/>
+    </row>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="C28" s="1"/>
+    </row>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B34" s="5"/>
+      <c r="C34" s="5"/>
+      <c r="D34" s="5"/>
+    </row>
+    <row r="35" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B35" s="6"/>
+      <c r="C35" s="6"/>
+      <c r="D35" s="6"/>
+    </row>
+    <row r="36" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B36" s="6"/>
+      <c r="C36" s="3"/>
+      <c r="D36" s="3"/>
+    </row>
+    <row r="37" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B37" s="6"/>
+      <c r="C37" s="3"/>
+      <c r="D37" s="3"/>
+    </row>
+    <row r="38" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B38" s="3"/>
+      <c r="C38" s="3"/>
+      <c r="D38" s="4"/>
+    </row>
+    <row r="39" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B39" s="6"/>
+      <c r="C39" s="3"/>
+      <c r="D39" s="4"/>
+    </row>
+    <row r="40" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B40" s="6"/>
+      <c r="C40" s="3"/>
+      <c r="D40" s="4"/>
+    </row>
+    <row r="41" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B41" s="6"/>
+      <c r="C41" s="3"/>
+      <c r="D41" s="4"/>
+    </row>
+    <row r="42" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B42" s="6"/>
+      <c r="C42" s="3"/>
+      <c r="D42" s="4"/>
+    </row>
+    <row r="43" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B43" s="6"/>
+      <c r="C43" s="3"/>
+      <c r="D43" s="4"/>
+    </row>
+    <row r="44" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B44" s="6"/>
+      <c r="C44" s="3"/>
+      <c r="D44" s="4"/>
+    </row>
+    <row r="45" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B45" s="6"/>
+      <c r="C45" s="3"/>
+      <c r="D45" s="4"/>
+    </row>
+    <row r="46" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B46" s="6"/>
+      <c r="C46" s="3"/>
+      <c r="D46" s="4"/>
+    </row>
+    <row r="47" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B47" s="6"/>
+      <c r="C47" s="3"/>
+      <c r="D47" s="4"/>
+    </row>
+    <row r="48" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B48" s="6"/>
+      <c r="C48" s="3"/>
+      <c r="D48" s="4"/>
+    </row>
+    <row r="49" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B49" s="6"/>
+      <c r="C49" s="3"/>
+      <c r="D49" s="4"/>
+    </row>
+    <row r="50" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B50" s="6"/>
+      <c r="C50" s="3"/>
+      <c r="D50" s="4"/>
+    </row>
+    <row r="51" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B51" s="6"/>
+      <c r="C51" s="3"/>
+      <c r="D51" s="4"/>
+    </row>
+    <row r="52" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B52" s="6"/>
+      <c r="C52" s="3"/>
+      <c r="D52" s="4"/>
+    </row>
+    <row r="53" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B53" s="6"/>
+      <c r="C53" s="3"/>
+      <c r="D53" s="4"/>
+    </row>
+    <row r="54" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B54" s="7"/>
+      <c r="C54" s="7"/>
+      <c r="D54" s="7"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="014f7f5d-144d-4041-bba0-be833a6b936c" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="014f7f5d-144d-4041-bba0-be833a6b936c" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1509,19 +1679,19 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{261ED46F-EA54-468D-AE56-6BB1C53F2697}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{11CA1BE4-1198-425C-85DD-E0B58ECAE203}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="014f7f5d-144d-4041-bba0-be833a6b936c"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{261ED46F-EA54-468D-AE56-6BB1C53F2697}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>